<commit_message>
fix bug when parse technology type
</commit_message>
<xml_diff>
--- a/app/static/template_events.xlsx
+++ b/app/static/template_events.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="55">
   <si>
     <t>Задание</t>
   </si>
@@ -142,6 +142,48 @@
   </si>
   <si>
     <t>High</t>
+  </si>
+  <si>
+    <t>Задание 7</t>
+  </si>
+  <si>
+    <t>Политика 7</t>
+  </si>
+  <si>
+    <t>promoall.docx</t>
+  </si>
+  <si>
+    <t>promotwo.docx</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Задание 8</t>
+  </si>
+  <si>
+    <t>Политика 8</t>
+  </si>
+  <si>
+    <t>catoo.jpg</t>
+  </si>
+  <si>
+    <t>catoo_reduced.jpg</t>
+  </si>
+  <si>
+    <t>Задание 9</t>
+  </si>
+  <si>
+    <t>Политика 9</t>
+  </si>
+  <si>
+    <t>evil_routes.rtf</t>
+  </si>
+  <si>
+    <t>routes.rtf</t>
+  </si>
+  <si>
+    <t>Accounting</t>
   </si>
 </sst>
 </file>
@@ -475,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K10"/>
+  <dimension ref="A2:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,6 +813,344 @@
         <v>28</v>
       </c>
     </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K22" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>